<commit_message>
Feat: nuevos controles añadidos
</commit_message>
<xml_diff>
--- a/errores.xlsx
+++ b/errores.xlsx
@@ -1,37 +1,154 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
+  <si>
+    <t>Archivo</t>
+  </si>
+  <si>
+    <t>Columna</t>
+  </si>
+  <si>
+    <t>Mensaje de error</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Población críticos</t>
+  </si>
+  <si>
+    <t>Inventario controles</t>
+  </si>
+  <si>
+    <t>RESPONSABLE FUNCIONAL</t>
+  </si>
+  <si>
+    <t>INFORME</t>
+  </si>
+  <si>
+    <t>CONCEPTO DEDUCIDO DEL INFORME</t>
+  </si>
+  <si>
+    <t>TIPO DE DATO</t>
+  </si>
+  <si>
+    <t>COMPONENTES</t>
+  </si>
+  <si>
+    <t>MÉTRICA EN INFORME</t>
+  </si>
+  <si>
+    <t>TIPO DE CONCEPTO</t>
+  </si>
+  <si>
+    <t>CRITICIDAD</t>
+  </si>
+  <si>
+    <t>ID CONTROLES</t>
+  </si>
+  <si>
+    <t>RESPONSABLE DE EJECUTAR EL CONTROL</t>
+  </si>
+  <si>
+    <t>TIPO DE CONTROL</t>
+  </si>
+  <si>
+    <t>MODO DE EJECUCIÓN</t>
+  </si>
+  <si>
+    <t>Se encontraron 84 registros con discrepancias.</t>
+  </si>
+  <si>
+    <t>Se encontraron 308 registros con discrepancias.</t>
+  </si>
+  <si>
+    <t>Se encontraron 2 valores no permitidos en 'INFORME'.</t>
+  </si>
+  <si>
+    <t>Se encontraron 1 valores duplicados.</t>
+  </si>
+  <si>
+    <t>No se encontraron los componentes, {68: ['Importe de la dotación sin ltfx'], 74: ['Importe de la dotación sin ltfx'], 75: ['Importe de la dotación sin ltfx'], 77: ['Importe de la dotación sin ltfx'], 84: ['COD_SIT_CONTA'], 91: ['Seguros de Vida Prima única'], 123: ['Riesgos Contingentes dudosos'], 137: ['VAL_NUM', 'VAL_DENO'], 141: ['VAL_NUM', 'VAL_DENO'], 194: ['Inversión Crediticia Bruta'], 197: ['Inversión Crediticia Bruta'], 200: ['Inversión Crediticia Bruta'], 203: ['Inversión Crediticia Bruta'], 204: ['Inversión Crediticia Bruta'], 211: ['Inversión Crediticia Bruta'], 219: ['Inversión Crediticia Bruta'], 220: ['Total Activos con cargas y sin cargas'], 223: ['Inversión Crediticia Bruta'], 265: ['MINUSVALÍAS NETAS'], 278: ['Otros ingresos\\gastos de explotación (dato presupuestado)'], 288: ['impacto en VE subida 200 pb', 'impacto en VE bajada 200 pb'], 311: ['Aportación  Nominal', 'Movimientos de coste sin movimiento de tesoreria'], 313: ['deposito'], 314: ['deposito'], 315: ['deposito'], 316: ['deposito'], 317: ['deposito'], 318: ['deposito'], 342: ['Nº de reclamaciones ante BDE (mes actual-1)', 'Nº de reclamaciones ante BDE  (mes actual-2)'], 355: ['Nivel de seguridad en  Activos en CPD en entornos Críticos que tienen vulnerabilidades críticas o altas con una antigüedad superior a 30 días'], 358: ['BAJAS REEST'], 361: ['Margen Financiero de gestión', 'Comisiones no financieras de gestión'], 486: ['Aportación  Nominal'], 536: ['mercado', 'tipooper', 'tiposaldo'], 537: ['mercado', 'tipooper', 'tiposaldo'], 538: ['mercado', 'tipooper', 'tiposaldo'], 539: ['mercado', 'tipooper', 'tiposaldo'], 610: ['Importe euros'], 611: ['Importe euros'], 635: ['Capital IRB\u200b'], 656: ['Importe euros'], 659: ['Importe euros'], 700: ['Importe de la dotación sin ltfx'], 710: ['Nº clientes comunicados y/o cancelados las relaciones mes N-1', 'Nº clientes comunicados y/o cancelados las relaciones mes N-2'], 744: ['COD_REG_ACT_MD', 'IND_01_BAJA_AC'], 745: ['codestadoac'], 778: ['Exposiciones en balance sujetas a riesgo de crédito (0070), Exposiciones fuera de balance sujetas a riesgo de crédito (0080), Importe de la exposición ponderada por riesgo después de aplicar los factores de apoyo (0220)'], 786: ['codestadoac']}, en la columna Concepto deducido del informe.</t>
+  </si>
+  <si>
+    <t>La columna 'MÉTRICA EN INFORME' tiene 2 valores vacíos.</t>
+  </si>
+  <si>
+    <t>Se encontraron 6 valores no permitidos en 'MÉTRICA EN INFORME'.</t>
+  </si>
+  <si>
+    <t>La columna 'ID CONTROLES' tiene 3 valores vacíos.</t>
+  </si>
+  <si>
+    <t>Se han encontrado las siguientes inconsistencias entre el ID y el modo de ejecución:      INFORME  ID DATO     ID CONTROLES ID existente TI  ...         Auxiliar Duplicados Aux Anna para ID de TI                                        concat_real                                    concat_esperada
+415  ISPAMAR      NaN  N2_A_INF_000954             NaN  ...  Coherencia funcionalN/AN/A                    NaN  8940 - Dirección de Personas8161 - Estructura ...  8940 - DIRECCIÓN DE PERSONAS8161 - Estructura ...
+416  ISPAMAR      NaN  N1_A_INF_000955             NaN  ...           CompletitudN/AN/A                    NaN  8940 - Dirección de Personas8161 - Estructura ...  8940 - DIRECCIÓN DE PERSONAS8161 - Estructura ...
+417  ISPAMAR      NaN  N1_A_INF_000956             NaN  ...    Valores permitidosN/AN/A                    NaN  8940 - Dirección de Personas8161 - Estructura ...  8940 - DIRECCIÓN DE PERSONAS8161 - Estructura ...
+[3 rows x 32 columns]</t>
+  </si>
+  <si>
+    <t>Se han encontrado las siguientes inconsistencias entre el ID y el tipo de control:       INFORME  ID DATO     ID CONTROLES  ... Aux Anna para ID de TI                                        concat_real                                    concat_esperada
+24    ISPAMAR      NaN  N3_M_INF_000865  ...                    NaN  8786 - DIRECCIÓN DE PLANIFICACIÓN FINANCIERA Y...  8786 - DIRECCIÓN DE PLANIFICACIÓN FINANCIERA Y...
+26        RAF      NaN  N3_M_INF_000872  ...                    NaN  8786 - DIRECCIÓN DE PLANIFICACIÓN FINANCIERA Y...  8786 - DIRECCIÓN DE PLANIFICACIÓN FINANCIERA Y...
+32        IRP      NaN  N3_M_INF_000771  ...                    NaN  8786 - DIRECCIÓN DE PLANIFICACIÓN FINANCIERA Y...  8786 - DIRECCIÓN DE PLANIFICACIÓN FINANCIERA Y...
+54    ISPAMAR      NaN  N3_M_INF_000938  ...                    NaN  8920 - DIRECCIÓN GENERAL FINANCIERA9051 - INFO...  8920 - DIRECCIÓN GENERAL FINANCIERA9051 - INFO...
+71      ICAAP      NaN  N3_M_INF_000785  ...                    NaN  8786 - DIRECCIÓN DE PLANIFICACIÓN FINANCIERA Y...  8786 - DIRECCIÓN DE PLANIFICACIÓN FINANCIERA Y...
+...       ...      ...              ...  ...                    ...                                                ...                                                ...
+1517  ISPAMAR      NaN  N3_M_INF_000867  ...                    NaN  8786 - DIRECCIÓN DE PLANIFICACIÓN FINANCIERA Y...  8786 - DIRECCIÓN DE PLANIFICACIÓN FINANCIERA Y...
+1520      RAF      NaN  N3_M_INF_001176  ...                    NaN  8900 - CONSEJO RECTOR PRESIDENTE7979 - SECRETA...  8900 - CONSEJO RECTOR PRESIDENTE7979 - SECRETA...
+1521      RAF      NaN  N3_M_INF_001177  ...                    NaN  8900 - CONSEJO RECTOR PRESIDENTE7979 - SECRETA...  8900 - CONSEJO RECTOR PRESIDENTE7979 - SECRETA...
+1522      RAF      NaN  N3_M_INF_001178  ...                    NaN  8900 - CONSEJO RECTOR PRESIDENTE7979 - SECRETA...  8900 - CONSEJO RECTOR PRESIDENTE7979 - SECRETA...
+1523      RAF      NaN  N3_M_INF_001175  ...                    NaN  8900 - CONSEJO RECTOR PRESIDENTE7979 - SECRETA...  8900 - CONSEJO RECTOR PRESIDENTE7979 - SECRETA...
+[176 rows x 32 columns]</t>
+  </si>
+  <si>
+    <t>Se han encontrado inconsistencias de ID entre informes. Se han guardado en 'errores_id_informe.xlsx'.</t>
+  </si>
+  <si>
+    <t>La columna 'RESPONSABLE DE EJECUTAR EL CONTROL' tiene 170 valores vacíos.</t>
+  </si>
+  <si>
+    <t>Se encontraron 157 valores no permitidos en 'TIPO DE CONTROL'.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +163,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,71 +479,397 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Archivo</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Columna</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Mensaje de error</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Población críticos</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>INFORME</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>La columna 'INFORME' tiene 3 valores vacíos.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Población críticos</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>INFORME</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>La columna 'NOMBRE DEL CONCEPTO' tiene 3 valores vacíos.</t>
-        </is>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>